<commit_message>
upd data, add models evaluation
</commit_message>
<xml_diff>
--- a/combat_losses.xlsx
+++ b/combat_losses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markiian_tsalyk/Desktop/russianInvasionAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887B6E06-8C8F-D54F-BD0A-8C37190A0A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B7927B-ABD5-FE46-B483-DACF82AE8801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15800" yWindow="520" windowWidth="13000" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="500" windowWidth="15120" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -123,6 +123,9 @@
   <si>
     <t>mobile SRBM system</t>
   </si>
+  <si>
+    <t>cruise missiles</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;/&quot;mm&quot;/&quot;yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -160,6 +163,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +215,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,10 +438,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L39" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView tabSelected="1" topLeftCell="M63" workbookViewId="0">
+      <selection activeCell="P70" sqref="P70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -443,10 +456,11 @@
     <col min="13" max="13" width="36.5" style="4" customWidth="1"/>
     <col min="14" max="14" width="24.6640625" style="4" customWidth="1"/>
     <col min="15" max="15" width="25" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="14.5" style="4"/>
+    <col min="16" max="16" width="18.5" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="14.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +506,11 @@
       <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1">
       <c r="A2" s="5">
         <f>DATE(2022, 2, 24)</f>
         <v>44616</v>
@@ -540,10 +557,13 @@
       <c r="O2" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A53" si="0">A2+1</f>
+        <f t="shared" ref="A3:A69" si="0">A2+1</f>
         <v>44617</v>
       </c>
       <c r="B3" s="4">
@@ -588,8 +608,11 @@
       <c r="O3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>44618</v>
@@ -636,8 +659,11 @@
       <c r="O4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>44619</v>
@@ -684,8 +710,11 @@
       <c r="O5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>44620</v>
@@ -732,8 +761,11 @@
       <c r="O6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>44621</v>
@@ -780,8 +812,11 @@
       <c r="O7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>44622</v>
@@ -828,8 +863,11 @@
       <c r="O8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>44623</v>
@@ -876,8 +914,11 @@
       <c r="O9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>44624</v>
@@ -924,8 +965,11 @@
       <c r="O10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>44625</v>
@@ -972,8 +1016,11 @@
       <c r="O11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>44626</v>
@@ -1020,8 +1067,11 @@
       <c r="O12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>44627</v>
@@ -1068,8 +1118,11 @@
       <c r="O13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>44628</v>
@@ -1116,8 +1169,11 @@
       <c r="O14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>44629</v>
@@ -1164,8 +1220,11 @@
       <c r="O15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>44630</v>
@@ -1212,8 +1271,11 @@
       <c r="O16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>44631</v>
@@ -1260,8 +1322,11 @@
       <c r="O17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>44632</v>
@@ -1308,8 +1373,11 @@
       <c r="O18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>44633</v>
@@ -1356,8 +1424,11 @@
       <c r="O19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>44634</v>
@@ -1404,8 +1475,11 @@
       <c r="O20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>44635</v>
@@ -1452,8 +1526,11 @@
       <c r="O21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>44636</v>
@@ -1500,8 +1577,11 @@
       <c r="O22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>44637</v>
@@ -1548,8 +1628,11 @@
       <c r="O23" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>44638</v>
@@ -1596,8 +1679,11 @@
       <c r="O24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>44639</v>
@@ -1644,8 +1730,11 @@
       <c r="O25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>44640</v>
@@ -1692,8 +1781,11 @@
       <c r="O26" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>44641</v>
@@ -1740,8 +1832,11 @@
       <c r="O27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>44642</v>
@@ -1788,8 +1883,11 @@
       <c r="O28" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>44643</v>
@@ -1836,8 +1934,11 @@
       <c r="O29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>44644</v>
@@ -1884,8 +1985,11 @@
       <c r="O30" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>44645</v>
@@ -1932,8 +2036,11 @@
       <c r="O31" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>44646</v>
@@ -1980,8 +2087,11 @@
       <c r="O32" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>44647</v>
@@ -2028,8 +2138,11 @@
       <c r="O33" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>44648</v>
@@ -2076,8 +2189,11 @@
       <c r="O34" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>44649</v>
@@ -2124,8 +2240,11 @@
       <c r="O35" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>44650</v>
@@ -2172,8 +2291,11 @@
       <c r="O36" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" customHeight="1">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>44651</v>
@@ -2220,8 +2342,11 @@
       <c r="O37" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" customHeight="1">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>44652</v>
@@ -2268,8 +2393,11 @@
       <c r="O38" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>44653</v>
@@ -2316,8 +2444,11 @@
       <c r="O39" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>44654</v>
@@ -2364,8 +2495,11 @@
       <c r="O40" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>44655</v>
@@ -2412,8 +2546,11 @@
       <c r="O41" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>44656</v>
@@ -2460,8 +2597,11 @@
       <c r="O42" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>44657</v>
@@ -2508,8 +2648,11 @@
       <c r="O43" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>44658</v>
@@ -2556,8 +2699,11 @@
       <c r="O44" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>44659</v>
@@ -2604,8 +2750,11 @@
       <c r="O45" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>44660</v>
@@ -2652,8 +2801,11 @@
       <c r="O46" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>44661</v>
@@ -2700,8 +2852,11 @@
       <c r="O47" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>44662</v>
@@ -2748,8 +2903,11 @@
       <c r="O48" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>44663</v>
@@ -2796,8 +2954,11 @@
       <c r="O49" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" customHeight="1">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>44664</v>
@@ -2844,8 +3005,11 @@
       <c r="O50" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" customHeight="1">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>44665</v>
@@ -2892,8 +3056,11 @@
       <c r="O51" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15.75" customHeight="1">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>44666</v>
@@ -2940,8 +3107,11 @@
       <c r="O52" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" ht="15.75" customHeight="1">
+      <c r="P52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="15.75" customHeight="1">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>44667</v>
@@ -2987,6 +3157,825 @@
       </c>
       <c r="O53" s="4">
         <v>4</v>
+      </c>
+      <c r="P53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A54" s="5">
+        <f t="shared" si="0"/>
+        <v>44668</v>
+      </c>
+      <c r="B54" s="4">
+        <v>20300</v>
+      </c>
+      <c r="C54" s="4">
+        <v>773</v>
+      </c>
+      <c r="D54" s="4">
+        <v>2002</v>
+      </c>
+      <c r="E54" s="4">
+        <v>376</v>
+      </c>
+      <c r="F54" s="4">
+        <v>127</v>
+      </c>
+      <c r="G54" s="4">
+        <v>66</v>
+      </c>
+      <c r="H54" s="4">
+        <v>165</v>
+      </c>
+      <c r="I54" s="4">
+        <v>146</v>
+      </c>
+      <c r="J54" s="4">
+        <v>1471</v>
+      </c>
+      <c r="K54" s="4">
+        <v>8</v>
+      </c>
+      <c r="L54" s="4">
+        <v>76</v>
+      </c>
+      <c r="M54" s="4">
+        <v>148</v>
+      </c>
+      <c r="N54" s="4">
+        <v>27</v>
+      </c>
+      <c r="O54" s="4">
+        <v>4</v>
+      </c>
+      <c r="P54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A55" s="5">
+        <f t="shared" si="0"/>
+        <v>44669</v>
+      </c>
+      <c r="B55" s="4">
+        <v>20600</v>
+      </c>
+      <c r="C55" s="4">
+        <v>790</v>
+      </c>
+      <c r="D55" s="4">
+        <v>2041</v>
+      </c>
+      <c r="E55" s="4">
+        <v>381</v>
+      </c>
+      <c r="F55" s="4">
+        <v>130</v>
+      </c>
+      <c r="G55" s="4">
+        <v>67</v>
+      </c>
+      <c r="H55" s="4">
+        <v>167</v>
+      </c>
+      <c r="I55" s="4">
+        <v>147</v>
+      </c>
+      <c r="J55" s="4">
+        <v>1487</v>
+      </c>
+      <c r="K55" s="4">
+        <v>8</v>
+      </c>
+      <c r="L55" s="4">
+        <v>76</v>
+      </c>
+      <c r="M55" s="4">
+        <v>155</v>
+      </c>
+      <c r="N55" s="4">
+        <v>27</v>
+      </c>
+      <c r="O55" s="4">
+        <v>4</v>
+      </c>
+      <c r="P55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A56" s="5">
+        <f t="shared" si="0"/>
+        <v>44670</v>
+      </c>
+      <c r="B56" s="4">
+        <v>20800</v>
+      </c>
+      <c r="C56" s="4">
+        <v>802</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2063</v>
+      </c>
+      <c r="E56" s="4">
+        <v>386</v>
+      </c>
+      <c r="F56" s="4">
+        <v>132</v>
+      </c>
+      <c r="G56" s="4">
+        <v>67</v>
+      </c>
+      <c r="H56" s="4">
+        <v>169</v>
+      </c>
+      <c r="I56" s="4">
+        <v>150</v>
+      </c>
+      <c r="J56" s="4">
+        <v>1495</v>
+      </c>
+      <c r="K56" s="4">
+        <v>8</v>
+      </c>
+      <c r="L56" s="4">
+        <v>76</v>
+      </c>
+      <c r="M56" s="4">
+        <v>158</v>
+      </c>
+      <c r="N56" s="4">
+        <v>27</v>
+      </c>
+      <c r="O56" s="4">
+        <v>4</v>
+      </c>
+      <c r="P56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A57" s="5">
+        <f t="shared" si="0"/>
+        <v>44671</v>
+      </c>
+      <c r="B57" s="4">
+        <v>20900</v>
+      </c>
+      <c r="C57" s="4">
+        <v>815</v>
+      </c>
+      <c r="D57" s="4">
+        <v>2087</v>
+      </c>
+      <c r="E57" s="4">
+        <v>391</v>
+      </c>
+      <c r="F57" s="4">
+        <v>136</v>
+      </c>
+      <c r="G57" s="4">
+        <v>67</v>
+      </c>
+      <c r="H57" s="4">
+        <v>171</v>
+      </c>
+      <c r="I57" s="4">
+        <v>150</v>
+      </c>
+      <c r="J57" s="4">
+        <v>1504</v>
+      </c>
+      <c r="K57" s="4">
+        <v>8</v>
+      </c>
+      <c r="L57" s="4">
+        <v>76</v>
+      </c>
+      <c r="M57" s="4">
+        <v>165</v>
+      </c>
+      <c r="N57" s="4">
+        <v>27</v>
+      </c>
+      <c r="O57" s="4">
+        <v>4</v>
+      </c>
+      <c r="P57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A58" s="5">
+        <f t="shared" si="0"/>
+        <v>44672</v>
+      </c>
+      <c r="B58" s="4">
+        <v>21000</v>
+      </c>
+      <c r="C58" s="4">
+        <v>829</v>
+      </c>
+      <c r="D58" s="4">
+        <v>2118</v>
+      </c>
+      <c r="E58" s="4">
+        <v>393</v>
+      </c>
+      <c r="F58" s="4">
+        <v>136</v>
+      </c>
+      <c r="G58" s="4">
+        <v>67</v>
+      </c>
+      <c r="H58" s="4">
+        <v>172</v>
+      </c>
+      <c r="I58" s="4">
+        <v>151</v>
+      </c>
+      <c r="J58" s="4">
+        <v>1508</v>
+      </c>
+      <c r="K58" s="4">
+        <v>8</v>
+      </c>
+      <c r="L58" s="4">
+        <v>76</v>
+      </c>
+      <c r="M58" s="4">
+        <v>166</v>
+      </c>
+      <c r="N58" s="4">
+        <v>27</v>
+      </c>
+      <c r="O58" s="4">
+        <v>4</v>
+      </c>
+      <c r="P58" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A59" s="5">
+        <f t="shared" si="0"/>
+        <v>44673</v>
+      </c>
+      <c r="B59" s="4">
+        <v>21200</v>
+      </c>
+      <c r="C59" s="4">
+        <v>838</v>
+      </c>
+      <c r="D59" s="4">
+        <v>2162</v>
+      </c>
+      <c r="E59" s="4">
+        <v>397</v>
+      </c>
+      <c r="F59" s="4">
+        <v>138</v>
+      </c>
+      <c r="G59" s="4">
+        <v>69</v>
+      </c>
+      <c r="H59" s="4">
+        <v>176</v>
+      </c>
+      <c r="I59" s="4">
+        <v>153</v>
+      </c>
+      <c r="J59" s="4">
+        <v>1523</v>
+      </c>
+      <c r="K59" s="4">
+        <v>8</v>
+      </c>
+      <c r="L59" s="4">
+        <v>76</v>
+      </c>
+      <c r="M59" s="4">
+        <v>172</v>
+      </c>
+      <c r="N59" s="4">
+        <v>27</v>
+      </c>
+      <c r="O59" s="4">
+        <v>4</v>
+      </c>
+      <c r="P59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A60" s="5">
+        <f t="shared" si="0"/>
+        <v>44674</v>
+      </c>
+      <c r="B60" s="4">
+        <v>21600</v>
+      </c>
+      <c r="C60" s="4">
+        <v>854</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2205</v>
+      </c>
+      <c r="E60" s="4">
+        <v>403</v>
+      </c>
+      <c r="F60" s="4">
+        <v>143</v>
+      </c>
+      <c r="G60" s="4">
+        <v>69</v>
+      </c>
+      <c r="H60" s="4">
+        <v>177</v>
+      </c>
+      <c r="I60" s="4">
+        <v>154</v>
+      </c>
+      <c r="J60" s="4">
+        <v>1543</v>
+      </c>
+      <c r="K60" s="4">
+        <v>8</v>
+      </c>
+      <c r="L60" s="4">
+        <v>76</v>
+      </c>
+      <c r="M60" s="4">
+        <v>182</v>
+      </c>
+      <c r="N60" s="4">
+        <v>27</v>
+      </c>
+      <c r="O60" s="4">
+        <v>4</v>
+      </c>
+      <c r="P60" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A61" s="5">
+        <f t="shared" si="0"/>
+        <v>44675</v>
+      </c>
+      <c r="B61" s="4">
+        <v>21800</v>
+      </c>
+      <c r="C61" s="4">
+        <v>873</v>
+      </c>
+      <c r="D61" s="4">
+        <v>2238</v>
+      </c>
+      <c r="E61" s="4">
+        <v>408</v>
+      </c>
+      <c r="F61" s="4">
+        <v>147</v>
+      </c>
+      <c r="G61" s="4">
+        <v>69</v>
+      </c>
+      <c r="H61" s="4">
+        <v>179</v>
+      </c>
+      <c r="I61" s="4">
+        <v>154</v>
+      </c>
+      <c r="J61" s="4">
+        <v>1557</v>
+      </c>
+      <c r="K61" s="4">
+        <v>8</v>
+      </c>
+      <c r="L61" s="4">
+        <v>76</v>
+      </c>
+      <c r="M61" s="4">
+        <v>191</v>
+      </c>
+      <c r="N61" s="4">
+        <v>28</v>
+      </c>
+      <c r="O61" s="4">
+        <v>4</v>
+      </c>
+      <c r="P61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A62" s="5">
+        <f t="shared" si="0"/>
+        <v>44676</v>
+      </c>
+      <c r="B62" s="4">
+        <v>21900</v>
+      </c>
+      <c r="C62" s="4">
+        <v>884</v>
+      </c>
+      <c r="D62" s="4">
+        <v>2258</v>
+      </c>
+      <c r="E62" s="4">
+        <v>411</v>
+      </c>
+      <c r="F62" s="4">
+        <v>149</v>
+      </c>
+      <c r="G62" s="4">
+        <v>69</v>
+      </c>
+      <c r="H62" s="4">
+        <v>181</v>
+      </c>
+      <c r="I62" s="4">
+        <v>154</v>
+      </c>
+      <c r="J62" s="4">
+        <v>1566</v>
+      </c>
+      <c r="K62" s="4">
+        <v>8</v>
+      </c>
+      <c r="L62" s="4">
+        <v>76</v>
+      </c>
+      <c r="M62" s="4">
+        <v>201</v>
+      </c>
+      <c r="N62" s="4">
+        <v>28</v>
+      </c>
+      <c r="O62" s="4">
+        <v>4</v>
+      </c>
+      <c r="P62" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A63" s="5">
+        <f t="shared" si="0"/>
+        <v>44677</v>
+      </c>
+      <c r="B63" s="4">
+        <v>22100</v>
+      </c>
+      <c r="C63" s="4">
+        <v>918</v>
+      </c>
+      <c r="D63" s="4">
+        <v>2308</v>
+      </c>
+      <c r="E63" s="4">
+        <v>416</v>
+      </c>
+      <c r="F63" s="4">
+        <v>149</v>
+      </c>
+      <c r="G63" s="4">
+        <v>69</v>
+      </c>
+      <c r="H63" s="4">
+        <v>184</v>
+      </c>
+      <c r="I63" s="4">
+        <v>154</v>
+      </c>
+      <c r="J63" s="4">
+        <v>1643</v>
+      </c>
+      <c r="K63" s="4">
+        <v>8</v>
+      </c>
+      <c r="L63" s="4">
+        <v>76</v>
+      </c>
+      <c r="M63" s="4">
+        <v>205</v>
+      </c>
+      <c r="N63" s="4">
+        <v>31</v>
+      </c>
+      <c r="O63" s="4">
+        <v>4</v>
+      </c>
+      <c r="P63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A64" s="5">
+        <f t="shared" si="0"/>
+        <v>44678</v>
+      </c>
+      <c r="B64" s="4">
+        <v>22400</v>
+      </c>
+      <c r="C64" s="4">
+        <v>939</v>
+      </c>
+      <c r="D64" s="4">
+        <v>2342</v>
+      </c>
+      <c r="E64" s="4">
+        <v>421</v>
+      </c>
+      <c r="F64" s="4">
+        <v>149</v>
+      </c>
+      <c r="G64" s="4">
+        <v>71</v>
+      </c>
+      <c r="H64" s="4">
+        <v>185</v>
+      </c>
+      <c r="I64" s="4">
+        <v>155</v>
+      </c>
+      <c r="J64" s="4">
+        <v>1666</v>
+      </c>
+      <c r="K64" s="4">
+        <v>8</v>
+      </c>
+      <c r="L64" s="4">
+        <v>76</v>
+      </c>
+      <c r="M64" s="4">
+        <v>207</v>
+      </c>
+      <c r="N64" s="4">
+        <v>31</v>
+      </c>
+      <c r="O64" s="4">
+        <v>4</v>
+      </c>
+      <c r="P64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A65" s="5">
+        <f t="shared" si="0"/>
+        <v>44679</v>
+      </c>
+      <c r="B65" s="4">
+        <v>22800</v>
+      </c>
+      <c r="C65" s="4">
+        <v>970</v>
+      </c>
+      <c r="D65" s="4">
+        <v>2389</v>
+      </c>
+      <c r="E65" s="4">
+        <v>431</v>
+      </c>
+      <c r="F65" s="4">
+        <v>151</v>
+      </c>
+      <c r="G65" s="4">
+        <v>72</v>
+      </c>
+      <c r="H65" s="4">
+        <v>187</v>
+      </c>
+      <c r="I65" s="4">
+        <v>155</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1688</v>
+      </c>
+      <c r="K65" s="4">
+        <v>8</v>
+      </c>
+      <c r="L65" s="4">
+        <v>76</v>
+      </c>
+      <c r="M65" s="4">
+        <v>215</v>
+      </c>
+      <c r="N65" s="4">
+        <v>31</v>
+      </c>
+      <c r="O65" s="4">
+        <v>4</v>
+      </c>
+      <c r="P65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A66" s="5">
+        <f t="shared" si="0"/>
+        <v>44680</v>
+      </c>
+      <c r="B66" s="4">
+        <v>23000</v>
+      </c>
+      <c r="C66" s="4">
+        <v>986</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2418</v>
+      </c>
+      <c r="E66" s="4">
+        <v>435</v>
+      </c>
+      <c r="F66" s="4">
+        <v>151</v>
+      </c>
+      <c r="G66" s="4">
+        <v>73</v>
+      </c>
+      <c r="H66" s="4">
+        <v>189</v>
+      </c>
+      <c r="I66" s="4">
+        <v>155</v>
+      </c>
+      <c r="J66" s="4">
+        <v>1695</v>
+      </c>
+      <c r="K66" s="4">
+        <v>8</v>
+      </c>
+      <c r="L66" s="4">
+        <v>76</v>
+      </c>
+      <c r="M66" s="4">
+        <v>229</v>
+      </c>
+      <c r="N66" s="4">
+        <v>31</v>
+      </c>
+      <c r="O66" s="4">
+        <v>4</v>
+      </c>
+      <c r="P66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A67" s="5">
+        <f t="shared" si="0"/>
+        <v>44681</v>
+      </c>
+      <c r="B67" s="4">
+        <v>23200</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1008</v>
+      </c>
+      <c r="D67" s="4">
+        <v>2445</v>
+      </c>
+      <c r="E67" s="4">
+        <v>436</v>
+      </c>
+      <c r="F67" s="4">
+        <v>151</v>
+      </c>
+      <c r="G67" s="4">
+        <v>77</v>
+      </c>
+      <c r="H67" s="4">
+        <v>190</v>
+      </c>
+      <c r="I67" s="4">
+        <v>155</v>
+      </c>
+      <c r="J67" s="4">
+        <v>1701</v>
+      </c>
+      <c r="K67" s="4">
+        <v>8</v>
+      </c>
+      <c r="L67" s="4">
+        <v>76</v>
+      </c>
+      <c r="M67" s="4">
+        <v>232</v>
+      </c>
+      <c r="N67" s="4">
+        <v>32</v>
+      </c>
+      <c r="O67" s="4">
+        <v>4</v>
+      </c>
+      <c r="P67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A68" s="5">
+        <f t="shared" si="0"/>
+        <v>44682</v>
+      </c>
+      <c r="B68" s="4">
+        <v>23500</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1026</v>
+      </c>
+      <c r="D68" s="4">
+        <v>2471</v>
+      </c>
+      <c r="E68" s="4">
+        <v>451</v>
+      </c>
+      <c r="F68" s="4">
+        <v>151</v>
+      </c>
+      <c r="G68" s="4">
+        <v>80</v>
+      </c>
+      <c r="H68" s="4">
+        <v>192</v>
+      </c>
+      <c r="I68" s="4">
+        <v>155</v>
+      </c>
+      <c r="J68" s="4">
+        <v>1796</v>
+      </c>
+      <c r="K68" s="4">
+        <v>8</v>
+      </c>
+      <c r="L68" s="4">
+        <v>76</v>
+      </c>
+      <c r="M68" s="4">
+        <v>245</v>
+      </c>
+      <c r="N68" s="4">
+        <v>32</v>
+      </c>
+      <c r="O68" s="4">
+        <v>4</v>
+      </c>
+      <c r="P68" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A69" s="5">
+        <f t="shared" si="0"/>
+        <v>44683</v>
+      </c>
+      <c r="B69" s="4">
+        <v>23800</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1048</v>
+      </c>
+      <c r="D69" s="4">
+        <v>2519</v>
+      </c>
+      <c r="E69" s="4">
+        <v>459</v>
+      </c>
+      <c r="F69" s="4">
+        <v>152</v>
+      </c>
+      <c r="G69" s="4">
+        <v>80</v>
+      </c>
+      <c r="H69" s="4">
+        <v>194</v>
+      </c>
+      <c r="I69" s="4">
+        <v>155</v>
+      </c>
+      <c r="J69" s="4">
+        <v>1824</v>
+      </c>
+      <c r="K69" s="4">
+        <v>8</v>
+      </c>
+      <c r="L69" s="4">
+        <v>76</v>
+      </c>
+      <c r="M69" s="4">
+        <v>271</v>
+      </c>
+      <c r="N69" s="4">
+        <v>38</v>
+      </c>
+      <c r="O69" s="4">
+        <v>4</v>
+      </c>
+      <c r="P69" s="4">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
develop arima model, upd data
</commit_message>
<xml_diff>
--- a/combat_losses.xlsx
+++ b/combat_losses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markiian_tsalyk/Desktop/russianInvasionAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D35492-883F-4C4D-8101-ED6A9B91AC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E76E4E-4BD4-B849-B591-32ADAC0D0AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="500" windowWidth="15120" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14720" yWindow="500" windowWidth="14080" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,10 +435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M58" workbookViewId="0">
-      <selection activeCell="O76" sqref="O76"/>
+    <sheetView tabSelected="1" topLeftCell="M76" workbookViewId="0">
+      <selection activeCell="O95" sqref="O95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A75" si="0">A2+1</f>
+        <f t="shared" ref="A3:A94" si="0">A2+1</f>
         <v>44617</v>
       </c>
       <c r="B3" s="4">
@@ -4054,6 +4054,918 @@
       </c>
       <c r="O75" s="4">
         <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A76" s="5">
+        <f t="shared" si="0"/>
+        <v>44690</v>
+      </c>
+      <c r="B76" s="4">
+        <v>25650</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1145</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2764</v>
+      </c>
+      <c r="E76" s="4">
+        <v>513</v>
+      </c>
+      <c r="F76" s="4">
+        <v>185</v>
+      </c>
+      <c r="G76" s="4">
+        <v>87</v>
+      </c>
+      <c r="H76" s="4">
+        <v>199</v>
+      </c>
+      <c r="I76" s="4">
+        <v>158</v>
+      </c>
+      <c r="J76" s="4">
+        <v>1970</v>
+      </c>
+      <c r="K76" s="4">
+        <v>12</v>
+      </c>
+      <c r="L76" s="4">
+        <v>377</v>
+      </c>
+      <c r="M76" s="4">
+        <v>41</v>
+      </c>
+      <c r="N76" s="4">
+        <v>4</v>
+      </c>
+      <c r="O76" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A77" s="5">
+        <f t="shared" si="0"/>
+        <v>44691</v>
+      </c>
+      <c r="B77" s="4">
+        <v>26000</v>
+      </c>
+      <c r="C77" s="4">
+        <v>1170</v>
+      </c>
+      <c r="D77" s="4">
+        <v>2808</v>
+      </c>
+      <c r="E77" s="4">
+        <v>519</v>
+      </c>
+      <c r="F77" s="4">
+        <v>185</v>
+      </c>
+      <c r="G77" s="4">
+        <v>87</v>
+      </c>
+      <c r="H77" s="4">
+        <v>199</v>
+      </c>
+      <c r="I77" s="4">
+        <v>158</v>
+      </c>
+      <c r="J77" s="4">
+        <v>1980</v>
+      </c>
+      <c r="K77" s="4">
+        <v>12</v>
+      </c>
+      <c r="L77" s="4">
+        <v>380</v>
+      </c>
+      <c r="M77" s="4">
+        <v>41</v>
+      </c>
+      <c r="N77" s="4">
+        <v>4</v>
+      </c>
+      <c r="O77" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A78" s="5">
+        <f t="shared" si="0"/>
+        <v>44692</v>
+      </c>
+      <c r="B78" s="4">
+        <v>26350</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1187</v>
+      </c>
+      <c r="D78" s="4">
+        <v>2856</v>
+      </c>
+      <c r="E78" s="4">
+        <v>528</v>
+      </c>
+      <c r="F78" s="4">
+        <v>185</v>
+      </c>
+      <c r="G78" s="4">
+        <v>87</v>
+      </c>
+      <c r="H78" s="4">
+        <v>199</v>
+      </c>
+      <c r="I78" s="4">
+        <v>160</v>
+      </c>
+      <c r="J78" s="4">
+        <v>1997</v>
+      </c>
+      <c r="K78" s="4">
+        <v>12</v>
+      </c>
+      <c r="L78" s="4">
+        <v>390</v>
+      </c>
+      <c r="M78" s="4">
+        <v>41</v>
+      </c>
+      <c r="N78" s="4">
+        <v>4</v>
+      </c>
+      <c r="O78" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A79" s="5">
+        <f t="shared" si="0"/>
+        <v>44693</v>
+      </c>
+      <c r="B79" s="4">
+        <v>26650</v>
+      </c>
+      <c r="C79" s="4">
+        <v>1195</v>
+      </c>
+      <c r="D79" s="4">
+        <v>2873</v>
+      </c>
+      <c r="E79" s="4">
+        <v>534</v>
+      </c>
+      <c r="F79" s="4">
+        <v>191</v>
+      </c>
+      <c r="G79" s="4">
+        <v>87</v>
+      </c>
+      <c r="H79" s="4">
+        <v>199</v>
+      </c>
+      <c r="I79" s="4">
+        <v>161</v>
+      </c>
+      <c r="J79" s="4">
+        <v>2019</v>
+      </c>
+      <c r="K79" s="4">
+        <v>13</v>
+      </c>
+      <c r="L79" s="4">
+        <v>398</v>
+      </c>
+      <c r="M79" s="4">
+        <v>41</v>
+      </c>
+      <c r="N79" s="4">
+        <v>4</v>
+      </c>
+      <c r="O79" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A80" s="5">
+        <f t="shared" si="0"/>
+        <v>44694</v>
+      </c>
+      <c r="B80" s="4">
+        <v>26900</v>
+      </c>
+      <c r="C80" s="4">
+        <v>1205</v>
+      </c>
+      <c r="D80" s="4">
+        <v>2900</v>
+      </c>
+      <c r="E80" s="4">
+        <v>542</v>
+      </c>
+      <c r="F80" s="4">
+        <v>193</v>
+      </c>
+      <c r="G80" s="4">
+        <v>88</v>
+      </c>
+      <c r="H80" s="4">
+        <v>200</v>
+      </c>
+      <c r="I80" s="4">
+        <v>162</v>
+      </c>
+      <c r="J80" s="4">
+        <v>2042</v>
+      </c>
+      <c r="K80" s="4">
+        <v>13</v>
+      </c>
+      <c r="L80" s="4">
+        <v>405</v>
+      </c>
+      <c r="M80" s="4">
+        <v>41</v>
+      </c>
+      <c r="N80" s="4">
+        <v>4</v>
+      </c>
+      <c r="O80" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A81" s="5">
+        <f t="shared" si="0"/>
+        <v>44695</v>
+      </c>
+      <c r="B81" s="4">
+        <v>27200</v>
+      </c>
+      <c r="C81" s="4">
+        <v>1218</v>
+      </c>
+      <c r="D81" s="4">
+        <v>2934</v>
+      </c>
+      <c r="E81" s="4">
+        <v>551</v>
+      </c>
+      <c r="F81" s="4">
+        <v>195</v>
+      </c>
+      <c r="G81" s="4">
+        <v>88</v>
+      </c>
+      <c r="H81" s="4">
+        <v>200</v>
+      </c>
+      <c r="I81" s="4">
+        <v>163</v>
+      </c>
+      <c r="J81" s="4">
+        <v>2059</v>
+      </c>
+      <c r="K81" s="4">
+        <v>13</v>
+      </c>
+      <c r="L81" s="4">
+        <v>411</v>
+      </c>
+      <c r="M81" s="4">
+        <v>42</v>
+      </c>
+      <c r="N81" s="4">
+        <v>4</v>
+      </c>
+      <c r="O81" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A82" s="5">
+        <f t="shared" si="0"/>
+        <v>44696</v>
+      </c>
+      <c r="B82" s="4">
+        <v>27400</v>
+      </c>
+      <c r="C82" s="4">
+        <v>1220</v>
+      </c>
+      <c r="D82" s="4">
+        <v>2958</v>
+      </c>
+      <c r="E82" s="4">
+        <v>555</v>
+      </c>
+      <c r="F82" s="4">
+        <v>195</v>
+      </c>
+      <c r="G82" s="4">
+        <v>89</v>
+      </c>
+      <c r="H82" s="4">
+        <v>200</v>
+      </c>
+      <c r="I82" s="4">
+        <v>164</v>
+      </c>
+      <c r="J82" s="4">
+        <v>2087</v>
+      </c>
+      <c r="K82" s="4">
+        <v>13</v>
+      </c>
+      <c r="L82" s="4">
+        <v>416</v>
+      </c>
+      <c r="M82" s="4">
+        <v>42</v>
+      </c>
+      <c r="N82" s="4">
+        <v>4</v>
+      </c>
+      <c r="O82" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A83" s="5">
+        <f t="shared" si="0"/>
+        <v>44697</v>
+      </c>
+      <c r="B83" s="4">
+        <v>27700</v>
+      </c>
+      <c r="C83" s="4">
+        <v>1228</v>
+      </c>
+      <c r="D83" s="4">
+        <v>2974</v>
+      </c>
+      <c r="E83" s="4">
+        <v>577</v>
+      </c>
+      <c r="F83" s="4">
+        <v>195</v>
+      </c>
+      <c r="G83" s="4">
+        <v>89</v>
+      </c>
+      <c r="H83" s="4">
+        <v>200</v>
+      </c>
+      <c r="I83" s="4">
+        <v>165</v>
+      </c>
+      <c r="J83" s="4">
+        <v>2101</v>
+      </c>
+      <c r="K83" s="4">
+        <v>13</v>
+      </c>
+      <c r="L83" s="4">
+        <v>427</v>
+      </c>
+      <c r="M83" s="4">
+        <v>42</v>
+      </c>
+      <c r="N83" s="4">
+        <v>4</v>
+      </c>
+      <c r="O83" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A84" s="5">
+        <f t="shared" si="0"/>
+        <v>44698</v>
+      </c>
+      <c r="B84" s="4">
+        <v>27900</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1235</v>
+      </c>
+      <c r="D84" s="4">
+        <v>3009</v>
+      </c>
+      <c r="E84" s="4">
+        <v>578</v>
+      </c>
+      <c r="F84" s="4">
+        <v>198</v>
+      </c>
+      <c r="G84" s="4">
+        <v>90</v>
+      </c>
+      <c r="H84" s="4">
+        <v>201</v>
+      </c>
+      <c r="I84" s="4">
+        <v>167</v>
+      </c>
+      <c r="J84" s="4">
+        <v>2109</v>
+      </c>
+      <c r="K84" s="4">
+        <v>13</v>
+      </c>
+      <c r="L84" s="4">
+        <v>436</v>
+      </c>
+      <c r="M84" s="4">
+        <v>43</v>
+      </c>
+      <c r="N84" s="4">
+        <v>4</v>
+      </c>
+      <c r="O84" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A85" s="5">
+        <f t="shared" si="0"/>
+        <v>44699</v>
+      </c>
+      <c r="B85" s="4">
+        <v>28300</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1251</v>
+      </c>
+      <c r="D85" s="4">
+        <v>3043</v>
+      </c>
+      <c r="E85" s="4">
+        <v>586</v>
+      </c>
+      <c r="F85" s="4">
+        <v>199</v>
+      </c>
+      <c r="G85" s="4">
+        <v>91</v>
+      </c>
+      <c r="H85" s="4">
+        <v>202</v>
+      </c>
+      <c r="I85" s="4">
+        <v>167</v>
+      </c>
+      <c r="J85" s="4">
+        <v>2137</v>
+      </c>
+      <c r="K85" s="4">
+        <v>13</v>
+      </c>
+      <c r="L85" s="4">
+        <v>441</v>
+      </c>
+      <c r="M85" s="4">
+        <v>43</v>
+      </c>
+      <c r="N85" s="4">
+        <v>4</v>
+      </c>
+      <c r="O85" s="4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A86" s="5">
+        <f t="shared" si="0"/>
+        <v>44700</v>
+      </c>
+      <c r="B86" s="4">
+        <v>28500</v>
+      </c>
+      <c r="C86" s="4">
+        <v>1254</v>
+      </c>
+      <c r="D86" s="4">
+        <v>3063</v>
+      </c>
+      <c r="E86" s="4">
+        <v>595</v>
+      </c>
+      <c r="F86" s="4">
+        <v>199</v>
+      </c>
+      <c r="G86" s="4">
+        <v>93</v>
+      </c>
+      <c r="H86" s="4">
+        <v>203</v>
+      </c>
+      <c r="I86" s="4">
+        <v>167</v>
+      </c>
+      <c r="J86" s="4">
+        <v>2157</v>
+      </c>
+      <c r="K86" s="4">
+        <v>13</v>
+      </c>
+      <c r="L86" s="4">
+        <v>455</v>
+      </c>
+      <c r="M86" s="4">
+        <v>43</v>
+      </c>
+      <c r="N86" s="4">
+        <v>4</v>
+      </c>
+      <c r="O86" s="4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A87" s="5">
+        <f t="shared" si="0"/>
+        <v>44701</v>
+      </c>
+      <c r="B87" s="4">
+        <v>28700</v>
+      </c>
+      <c r="C87" s="4">
+        <v>1263</v>
+      </c>
+      <c r="D87" s="4">
+        <v>3090</v>
+      </c>
+      <c r="E87" s="4">
+        <v>596</v>
+      </c>
+      <c r="F87" s="4">
+        <v>200</v>
+      </c>
+      <c r="G87" s="4">
+        <v>93</v>
+      </c>
+      <c r="H87" s="4">
+        <v>204</v>
+      </c>
+      <c r="I87" s="4">
+        <v>168</v>
+      </c>
+      <c r="J87" s="4">
+        <v>2162</v>
+      </c>
+      <c r="K87" s="4">
+        <v>13</v>
+      </c>
+      <c r="L87" s="4">
+        <v>460</v>
+      </c>
+      <c r="M87" s="4">
+        <v>43</v>
+      </c>
+      <c r="N87" s="4">
+        <v>4</v>
+      </c>
+      <c r="O87" s="4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A88" s="5">
+        <f t="shared" si="0"/>
+        <v>44702</v>
+      </c>
+      <c r="B88" s="4">
+        <v>28850</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1278</v>
+      </c>
+      <c r="D88" s="4">
+        <v>3116</v>
+      </c>
+      <c r="E88" s="4">
+        <v>596</v>
+      </c>
+      <c r="F88" s="4">
+        <v>201</v>
+      </c>
+      <c r="G88" s="4">
+        <v>93</v>
+      </c>
+      <c r="H88" s="4">
+        <v>204</v>
+      </c>
+      <c r="I88" s="4">
+        <v>169</v>
+      </c>
+      <c r="J88" s="4">
+        <v>2178</v>
+      </c>
+      <c r="K88" s="4">
+        <v>13</v>
+      </c>
+      <c r="L88" s="4">
+        <v>462</v>
+      </c>
+      <c r="M88" s="4">
+        <v>43</v>
+      </c>
+      <c r="N88" s="4">
+        <v>4</v>
+      </c>
+      <c r="O88" s="4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A89" s="5">
+        <f t="shared" si="0"/>
+        <v>44703</v>
+      </c>
+      <c r="B89" s="4">
+        <v>29050</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1285</v>
+      </c>
+      <c r="D89" s="4">
+        <v>3141</v>
+      </c>
+      <c r="E89" s="4">
+        <v>599</v>
+      </c>
+      <c r="F89" s="4">
+        <v>201</v>
+      </c>
+      <c r="G89" s="4">
+        <v>93</v>
+      </c>
+      <c r="H89" s="4">
+        <v>204</v>
+      </c>
+      <c r="I89" s="4">
+        <v>170</v>
+      </c>
+      <c r="J89" s="4">
+        <v>2194</v>
+      </c>
+      <c r="K89" s="4">
+        <v>13</v>
+      </c>
+      <c r="L89" s="4">
+        <v>470</v>
+      </c>
+      <c r="M89" s="4">
+        <v>43</v>
+      </c>
+      <c r="N89" s="4">
+        <v>4</v>
+      </c>
+      <c r="O89" s="4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A90" s="5">
+        <f t="shared" si="0"/>
+        <v>44704</v>
+      </c>
+      <c r="B90" s="4">
+        <v>29200</v>
+      </c>
+      <c r="C90" s="4">
+        <v>1293</v>
+      </c>
+      <c r="D90" s="4">
+        <v>3166</v>
+      </c>
+      <c r="E90" s="4">
+        <v>604</v>
+      </c>
+      <c r="F90" s="4">
+        <v>201</v>
+      </c>
+      <c r="G90" s="4">
+        <v>93</v>
+      </c>
+      <c r="H90" s="4">
+        <v>204</v>
+      </c>
+      <c r="I90" s="4">
+        <v>170</v>
+      </c>
+      <c r="J90" s="4">
+        <v>2206</v>
+      </c>
+      <c r="K90" s="4">
+        <v>13</v>
+      </c>
+      <c r="L90" s="4">
+        <v>476</v>
+      </c>
+      <c r="M90" s="4">
+        <v>43</v>
+      </c>
+      <c r="N90" s="4">
+        <v>4</v>
+      </c>
+      <c r="O90" s="4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A91" s="5">
+        <f t="shared" si="0"/>
+        <v>44705</v>
+      </c>
+      <c r="B91" s="4">
+        <v>29350</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1302</v>
+      </c>
+      <c r="D91" s="4">
+        <v>3194</v>
+      </c>
+      <c r="E91" s="4">
+        <v>606</v>
+      </c>
+      <c r="F91" s="4">
+        <v>201</v>
+      </c>
+      <c r="G91" s="4">
+        <v>93</v>
+      </c>
+      <c r="H91" s="4">
+        <v>205</v>
+      </c>
+      <c r="I91" s="4">
+        <v>170</v>
+      </c>
+      <c r="J91" s="4">
+        <v>2213</v>
+      </c>
+      <c r="K91" s="4">
+        <v>13</v>
+      </c>
+      <c r="L91" s="4">
+        <v>480</v>
+      </c>
+      <c r="M91" s="4">
+        <v>43</v>
+      </c>
+      <c r="N91" s="4">
+        <v>4</v>
+      </c>
+      <c r="O91" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A92" s="5">
+        <f t="shared" si="0"/>
+        <v>44706</v>
+      </c>
+      <c r="B92" s="4">
+        <v>29450</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1305</v>
+      </c>
+      <c r="D92" s="4">
+        <v>3213</v>
+      </c>
+      <c r="E92" s="4">
+        <v>606</v>
+      </c>
+      <c r="F92" s="4">
+        <v>201</v>
+      </c>
+      <c r="G92" s="4">
+        <v>93</v>
+      </c>
+      <c r="H92" s="4">
+        <v>206</v>
+      </c>
+      <c r="I92" s="4">
+        <v>170</v>
+      </c>
+      <c r="J92" s="4">
+        <v>2217</v>
+      </c>
+      <c r="K92" s="4">
+        <v>13</v>
+      </c>
+      <c r="L92" s="4">
+        <v>491</v>
+      </c>
+      <c r="M92" s="4">
+        <v>44</v>
+      </c>
+      <c r="N92" s="4">
+        <v>4</v>
+      </c>
+      <c r="O92" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A93" s="5">
+        <f t="shared" si="0"/>
+        <v>44707</v>
+      </c>
+      <c r="B93" s="4">
+        <v>29600</v>
+      </c>
+      <c r="C93" s="4">
+        <v>1315</v>
+      </c>
+      <c r="D93" s="4">
+        <v>3235</v>
+      </c>
+      <c r="E93" s="4">
+        <v>617</v>
+      </c>
+      <c r="F93" s="4">
+        <v>201</v>
+      </c>
+      <c r="G93" s="4">
+        <v>93</v>
+      </c>
+      <c r="H93" s="4">
+        <v>206</v>
+      </c>
+      <c r="I93" s="4">
+        <v>170</v>
+      </c>
+      <c r="J93" s="4">
+        <v>2225</v>
+      </c>
+      <c r="K93" s="4">
+        <v>13</v>
+      </c>
+      <c r="L93" s="4">
+        <v>502</v>
+      </c>
+      <c r="M93" s="4">
+        <v>47</v>
+      </c>
+      <c r="N93" s="4">
+        <v>4</v>
+      </c>
+      <c r="O93" s="4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A94" s="5">
+        <f t="shared" si="0"/>
+        <v>44708</v>
+      </c>
+      <c r="B94" s="4">
+        <v>29750</v>
+      </c>
+      <c r="C94" s="4">
+        <v>1322</v>
+      </c>
+      <c r="D94" s="4">
+        <v>3246</v>
+      </c>
+      <c r="E94" s="4">
+        <v>623</v>
+      </c>
+      <c r="F94" s="4">
+        <v>201</v>
+      </c>
+      <c r="G94" s="4">
+        <v>93</v>
+      </c>
+      <c r="H94" s="4">
+        <v>206</v>
+      </c>
+      <c r="I94" s="4">
+        <v>170</v>
+      </c>
+      <c r="J94" s="4">
+        <v>2226</v>
+      </c>
+      <c r="K94" s="4">
+        <v>13</v>
+      </c>
+      <c r="L94" s="4">
+        <v>503</v>
+      </c>
+      <c r="M94" s="4">
+        <v>48</v>
+      </c>
+      <c r="N94" s="4">
+        <v>4</v>
+      </c>
+      <c r="O94" s="4">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
developed forecasting, upd data
</commit_message>
<xml_diff>
--- a/combat_losses.xlsx
+++ b/combat_losses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markiian_tsalyk/Desktop/russianInvasionAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E76E4E-4BD4-B849-B591-32ADAC0D0AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8014252B-E07D-3C43-8667-BC60B6EA7AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14720" yWindow="500" windowWidth="14080" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,10 +435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M76" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95"/>
+    <sheetView tabSelected="1" topLeftCell="M80" workbookViewId="0">
+      <selection activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A94" si="0">A2+1</f>
+        <f t="shared" ref="A3:A97" si="0">A2+1</f>
         <v>44617</v>
       </c>
       <c r="B3" s="4">
@@ -4966,6 +4966,150 @@
       </c>
       <c r="O94" s="4">
         <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A95" s="5">
+        <f t="shared" si="0"/>
+        <v>44709</v>
+      </c>
+      <c r="B95" s="4">
+        <v>30000</v>
+      </c>
+      <c r="C95" s="4">
+        <v>1330</v>
+      </c>
+      <c r="D95" s="4">
+        <v>3258</v>
+      </c>
+      <c r="E95" s="4">
+        <v>628</v>
+      </c>
+      <c r="F95" s="4">
+        <v>203</v>
+      </c>
+      <c r="G95" s="4">
+        <v>93</v>
+      </c>
+      <c r="H95" s="4">
+        <v>207</v>
+      </c>
+      <c r="I95" s="4">
+        <v>174</v>
+      </c>
+      <c r="J95" s="4">
+        <v>2226</v>
+      </c>
+      <c r="K95" s="4">
+        <v>13</v>
+      </c>
+      <c r="L95" s="4">
+        <v>503</v>
+      </c>
+      <c r="M95" s="4">
+        <v>48</v>
+      </c>
+      <c r="N95" s="4">
+        <v>4</v>
+      </c>
+      <c r="O95" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A96" s="5">
+        <f t="shared" si="0"/>
+        <v>44710</v>
+      </c>
+      <c r="B96" s="4">
+        <v>30150</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1338</v>
+      </c>
+      <c r="D96" s="4">
+        <v>3270</v>
+      </c>
+      <c r="E96" s="4">
+        <v>631</v>
+      </c>
+      <c r="F96" s="4">
+        <v>203</v>
+      </c>
+      <c r="G96" s="4">
+        <v>93</v>
+      </c>
+      <c r="H96" s="4">
+        <v>207</v>
+      </c>
+      <c r="I96" s="4">
+        <v>174</v>
+      </c>
+      <c r="J96" s="4">
+        <v>2240</v>
+      </c>
+      <c r="K96" s="4">
+        <v>13</v>
+      </c>
+      <c r="L96" s="4">
+        <v>504</v>
+      </c>
+      <c r="M96" s="4">
+        <v>48</v>
+      </c>
+      <c r="N96" s="4">
+        <v>4</v>
+      </c>
+      <c r="O96" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A97" s="5">
+        <f t="shared" si="0"/>
+        <v>44711</v>
+      </c>
+      <c r="B97" s="4">
+        <v>30350</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1349</v>
+      </c>
+      <c r="D97" s="4">
+        <v>3282</v>
+      </c>
+      <c r="E97" s="4">
+        <v>643</v>
+      </c>
+      <c r="F97" s="4">
+        <v>205</v>
+      </c>
+      <c r="G97" s="4">
+        <v>93</v>
+      </c>
+      <c r="H97" s="4">
+        <v>207</v>
+      </c>
+      <c r="I97" s="4">
+        <v>174</v>
+      </c>
+      <c r="J97" s="4">
+        <v>2258</v>
+      </c>
+      <c r="K97" s="4">
+        <v>13</v>
+      </c>
+      <c r="L97" s="4">
+        <v>507</v>
+      </c>
+      <c r="M97" s="4">
+        <v>48</v>
+      </c>
+      <c r="N97" s="4">
+        <v>4</v>
+      </c>
+      <c r="O97" s="4">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>